<commit_message>
Fixed bugs and modified code for better performance and accuracy
</commit_message>
<xml_diff>
--- a/model_performance.xlsx
+++ b/model_performance.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_2B59D2BFD3C0D25C6F9A251159B790B06BD9FB29" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05E9E812-50BB-4044-A76A-F0460C6B5AD1}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_2B59D2BFD3505D60FF1A3F1159F7B8325733F87F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD50A822-E8CD-42B5-B799-95DBD645823F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="22">
   <si>
     <t>Script</t>
   </si>
@@ -52,52 +52,22 @@
     <t>hf_transformers_causallm_gemma2b_cpu.py</t>
   </si>
   <si>
-    <t>hf_transformers_causallm_gemma2b_flash_attention2.py</t>
-  </si>
-  <si>
-    <t>hf_transformers_causallm_gemma2b_gpu_4bit.py</t>
-  </si>
-  <si>
-    <t>hf_transformers_causallm_gemma2b_gpu_bfloat16.py</t>
-  </si>
-  <si>
-    <t>hf_transformers_causallm_gemma2b_gpu_float16.py</t>
-  </si>
-  <si>
-    <t>hf_transformers_causallm_gemma2b_gpu_int8.py</t>
-  </si>
-  <si>
-    <t>hf_transformers_causallm_gemma2b_gpu.py</t>
-  </si>
-  <si>
-    <t>llama_gguf_minicpmo.py</t>
-  </si>
-  <si>
-    <t>openbmb/MiniCPM-o-2_6-gguf</t>
+    <t>google/gemma-2b</t>
   </si>
   <si>
     <t>cpu</t>
   </si>
   <si>
+    <t>2.51</t>
+  </si>
+  <si>
+    <t>20.08</t>
+  </si>
+  <si>
+    <t>llama_gguf_gemma2b.py</t>
+  </si>
+  <si>
     <t>0.00</t>
-  </si>
-  <si>
-    <t>5.44</t>
-  </si>
-  <si>
-    <t>hf_transformers_pipeline_gemma2b.py</t>
-  </si>
-  <si>
-    <t>google/gemma-2b</t>
-  </si>
-  <si>
-    <t>cuda</t>
-  </si>
-  <si>
-    <t>2.51</t>
-  </si>
-  <si>
-    <t>15.07</t>
   </si>
 </sst>
 </file>
@@ -460,14 +430,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.5625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.00390625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.73828125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.3203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.71484375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.69140625" bestFit="1" customWidth="1"/>
@@ -502,81 +474,46 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>27.39</v>
+      </c>
+      <c r="E2">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D3">
+        <v>115.31</v>
+      </c>
+      <c r="E3">
+        <v>95.26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9">
-        <v>60.73</v>
-      </c>
-      <c r="E9">
-        <v>54.82</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10">
-        <v>48.77</v>
-      </c>
-      <c r="E10">
-        <v>29.6</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved the model inference with torch.inference_mode()
</commit_message>
<xml_diff>
--- a/model_performance.xlsx
+++ b/model_performance.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_2B59D2BFD3505D60FF1A3F1159F7B8325733F87F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD50A822-E8CD-42B5-B799-95DBD645823F}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_2B59D2BFD3505D60FF1A3F1159F7B8325733F87F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54BE54BD-3A85-4117-B5DC-DACD9E679561}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>Script</t>
   </si>
@@ -64,10 +64,34 @@
     <t>20.08</t>
   </si>
   <si>
+    <t>hf_transformers_causallm_gemma2b_gpu_4bit.py</t>
+  </si>
+  <si>
+    <t>cuda</t>
+  </si>
+  <si>
+    <t>1.52</t>
+  </si>
+  <si>
+    <t>hf_transformers_causallm_gemma2b_gpu_bfloat16.py</t>
+  </si>
+  <si>
+    <t>hf_transformers_causallm_gemma2b_gpu_float16.py</t>
+  </si>
+  <si>
+    <t>hf_transformers_causallm_gemma2b_gpu_int8.py</t>
+  </si>
+  <si>
+    <t>hf_transformers_causallm_gemma2b_gpu.py</t>
+  </si>
+  <si>
     <t>llama_gguf_gemma2b.py</t>
   </si>
   <si>
     <t>0.00</t>
+  </si>
+  <si>
+    <t>hf_transformers_pipeline_gemma2b.py</t>
   </si>
 </sst>
 </file>
@@ -430,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -501,18 +525,144 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>16.46</v>
+      </c>
+      <c r="E3">
+        <v>2.64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>27.36</v>
+      </c>
+      <c r="E4">
+        <v>13.79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>52.64</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>44.44</v>
+      </c>
+      <c r="E7">
+        <v>30.77</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D8">
         <v>115.31</v>
       </c>
-      <c r="E3">
+      <c r="E8">
         <v>95.26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="D9">
+        <v>73.12</v>
+      </c>
+      <c r="E9">
+        <v>63.77</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>